<commit_message>
Added the alarming to Base Project Some Method names were reduced do to size of path
</commit_message>
<xml_diff>
--- a/PML_Base_PLC_Project/PLC_PML/Base/01_PML/98_EventDefinitions/PMLBase_TMCTemplate.xlsx
+++ b/PML_Base_PLC_Project/PLC_PML/Base/01_PML/98_EventDefinitions/PMLBase_TMCTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beckhoff_Work\github\PML_Base_PLC_BenS_Development\PML_Base_PLC_Project\PLC_PML\Base\01_PML\98_EventDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KeithBa\source\repos\BeckhoffUS\PML_Base_Development\pml-base-plc-development\PML_Base_PLC_Project\PLC_PML\Base\01_PML\98_EventDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9798694-E8D4-4FFA-847D-0CC80E3D3926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7EAD39-D043-40B8-A7A3-C5A0547CC2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1155" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="226">
   <si>
     <t>Key</t>
   </si>
@@ -708,15 +708,6 @@
     <t>DT_BaseAlarms_Event_ComponentError</t>
   </si>
   <si>
-    <t>SubmoduleAborted</t>
-  </si>
-  <si>
-    <t>DT_BaseAlarms_Event_SubmoduleAborted</t>
-  </si>
-  <si>
-    <t>{0} - Submodule aborted during operation - Submodule Name: {1}</t>
-  </si>
-  <si>
     <t>{0} - Component error in module during operation - Component Name: {1}</t>
   </si>
   <si>
@@ -739,6 +730,18 @@
   </si>
   <si>
     <t>{DD613D9B-2D36-4D21-9065-3987280E65BE}</t>
+  </si>
+  <si>
+    <t>SubModuleError</t>
+  </si>
+  <si>
+    <t>DT_BaseAlarms_Event_SubModuleError</t>
+  </si>
+  <si>
+    <t>{0} - SubModule Error during operation - Submodule Name: {1}</t>
+  </si>
+  <si>
+    <t>{FA67A42A-DB7C-49E5-90EF-5F1EF533D41D}</t>
   </si>
 </sst>
 </file>
@@ -919,8 +922,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B17" totalsRowShown="0">
-  <autoFilter ref="A1:B17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B18" totalsRowShown="0">
+  <autoFilter ref="A1:B18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="EventClass"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Guid"/>
@@ -1250,11 +1253,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1523,7 @@
         <v>178</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E21" t="s">
         <v>125</v>
@@ -1792,10 +1795,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C46" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1803,15 +1806,15 @@
         <v>213</v>
       </c>
       <c r="C47" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C48" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +1876,7 @@
         <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
         <v>164</v>
@@ -1884,7 +1887,7 @@
         <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
         <v>159</v>
@@ -2037,11 +2040,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2091,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2098,7 +2101,7 @@
       </c>
       <c r="D3" t="str" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P5),LEN(CELL("filename",P5))-FIND("]",CELL("filename",P5))),"_Event_", BaseAlarms[[#This Row],[Name]])</f>
-        <v>DT_BaseAlarms_Event_SubmoduleAborted</v>
+        <v>DT_BaseAlarms_Event_SubModuleError</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2118,7 +2121,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2877,7 +2880,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -3022,7 +3025,15 @@
         <v>162</v>
       </c>
       <c r="B17" t="s">
-        <v>219</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3164,10 +3175,10 @@
         <v>162</v>
       </c>
       <c r="B7">
-        <v>-112183645</v>
+        <v>-668640524</v>
       </c>
       <c r="C7">
-        <v>-1061140768</v>
+        <v>-1957413921</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added back the ProductionData and Interfaces under Base Cleaned up error
</commit_message>
<xml_diff>
--- a/PML_Base_PLC_Project/PLC_PML/Base/01_PML/98_EventDefinitions/PMLBase_TMCTemplate.xlsx
+++ b/PML_Base_PLC_Project/PLC_PML/Base/01_PML/98_EventDefinitions/PMLBase_TMCTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KeithBa\source\repos\BeckhoffUS\PML_Base_Development\pml-base-plc-development\PML_Base_PLC_Project\PLC_PML\Base\01_PML\98_EventDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7EAD39-D043-40B8-A7A3-C5A0547CC2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAADC20-FED3-454F-A16D-71D2612DCFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1155" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,11 @@
     <sheet name="System" sheetId="7" r:id="rId3"/>
     <sheet name="BaseAlarms" sheetId="16" r:id="rId4"/>
     <sheet name="PMLAlarms" sheetId="15" r:id="rId5"/>
-    <sheet name="TemplateEventClass" sheetId="8" r:id="rId6"/>
-    <sheet name="HiddenDataTypes" sheetId="5" r:id="rId7"/>
-    <sheet name="Helper" sheetId="4" state="hidden" r:id="rId8"/>
-    <sheet name="EventClassHashTable" sheetId="13" state="hidden" r:id="rId9"/>
+    <sheet name="ProductionData" sheetId="17" r:id="rId6"/>
+    <sheet name="TemplateEventClass" sheetId="8" r:id="rId7"/>
+    <sheet name="HiddenDataTypes" sheetId="5" r:id="rId8"/>
+    <sheet name="Helper" sheetId="4" state="hidden" r:id="rId9"/>
+    <sheet name="EventClassHashTable" sheetId="13" state="hidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="241">
   <si>
     <t>Key</t>
   </si>
@@ -742,6 +743,51 @@
   </si>
   <si>
     <t>{FA67A42A-DB7C-49E5-90EF-5F1EF533D41D}</t>
+  </si>
+  <si>
+    <t>ProductionData</t>
+  </si>
+  <si>
+    <t>{F25DAB20-2AFF-4DFA-93A2-6BEFAF5EA238}</t>
+  </si>
+  <si>
+    <t>DT_ProductionData</t>
+  </si>
+  <si>
+    <t>TargetRateChanged</t>
+  </si>
+  <si>
+    <t>ShiftCompleted</t>
+  </si>
+  <si>
+    <t>BehindScheduleAcceptable</t>
+  </si>
+  <si>
+    <t>BehindScheduleWarning</t>
+  </si>
+  <si>
+    <t>DT_ProductionData_Event_TargetRateChanged</t>
+  </si>
+  <si>
+    <t>DT_ProductionData_Event_ShiftCompleted</t>
+  </si>
+  <si>
+    <t>DT_ProductionData_Event_BehindScheduleAcceptable</t>
+  </si>
+  <si>
+    <t>DT_ProductionData_Event_BehindScheduleWarning</t>
+  </si>
+  <si>
+    <t>{0} - Target production rate updated - New Rate: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Production shoft completed - Products Produced: {1}</t>
+  </si>
+  <si>
+    <t>{0} - Production is behind schedule within 'Acceptable' window - Rate required to meet shift taraget: {1} PPM</t>
+  </si>
+  <si>
+    <t>{0} - Production is behind schedule within 'Warning' window - Rate required to meet shift taraget: {1} PPM</t>
   </si>
 </sst>
 </file>
@@ -783,7 +829,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -832,8 +885,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Translations" displayName="Translations" ref="A1:K48" totalsRowShown="0">
-  <autoFilter ref="A1:K48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Translations" displayName="Translations" ref="A1:K52" totalsRowShown="0">
+  <autoFilter ref="A1:K52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Key"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="German (1031)"/>
@@ -851,9 +904,21 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="EventClassHashTable" displayName="EventClassHashTable" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="EventClassHash"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TranslationHash"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="EventClasses" displayName="EventClasses" ref="A1:E35" totalsRowShown="0">
-  <autoFilter ref="A1:E35" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="EventClasses" displayName="EventClasses" ref="A1:E36" totalsRowShown="0">
+  <autoFilter ref="A1:E36" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Namespace"/>
@@ -908,6 +973,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B17DE993-EBB5-4913-85C6-EF3CD0CC60F7}" name="ProductionData" displayName="ProductionData" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C578FCC0-4483-49C2-BDE1-CE0EFA70873A}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{ED15CA3E-178B-4DB9-80E9-BC9D704C511B}" name="Id"/>
+    <tableColumn id="3" xr3:uid="{5516D589-2F4F-4CAF-8C06-363D4DB7D43C}" name="Severity"/>
+    <tableColumn id="4" xr3:uid="{A25F1357-B173-4FE4-909E-37589E690879}" name="Display Text"/>
+    <tableColumn id="5" xr3:uid="{F8D1B4BE-62F4-4CDC-9020-9FF1B4F614CF}" name="Comment"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="TemplateEventClass" displayName="TemplateEventClass" ref="A1:E5" totalsRowShown="0">
   <autoFilter ref="A1:E5" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="5">
@@ -921,7 +1000,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="HiddenDataTypes" displayName="HiddenDataTypes" ref="A1:B18" totalsRowShown="0">
   <autoFilter ref="A1:B18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
@@ -932,23 +1011,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Helper" displayName="Helper" ref="A1:A6" totalsRowShown="0">
   <autoFilter ref="A1:A6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Severity"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="EventClassHashTable" displayName="EventClassHashTable" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="EventClassHash"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TranslationHash"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1251,13 +1318,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,6 +1884,38 @@
         <v>219</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>233</v>
+      </c>
+      <c r="C49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>235</v>
+      </c>
+      <c r="C51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1826,9 +1925,160 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>1998170941</v>
+      </c>
+      <c r="C2">
+        <v>-1925411841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>1054446003</v>
+      </c>
+      <c r="C3">
+        <v>662966212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>1691620521</v>
+      </c>
+      <c r="C4">
+        <v>1845685619</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>2038111688</v>
+      </c>
+      <c r="C5">
+        <v>46465576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>-1810971161</v>
+      </c>
+      <c r="C6">
+        <v>1659002869</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7">
+        <v>-668640524</v>
+      </c>
+      <c r="C7">
+        <v>-1957413921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8">
+        <v>-1476574130</v>
+      </c>
+      <c r="C8">
+        <v>-97488637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9">
+        <v>1259079353</v>
+      </c>
+      <c r="C9">
+        <v>-1307371275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10">
+        <v>1688958672</v>
+      </c>
+      <c r="C10">
+        <v>-1307371275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11">
+        <v>-1825382818</v>
+      </c>
+      <c r="C11">
+        <v>-1307371275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12">
+        <v>905478954</v>
+      </c>
+      <c r="C12">
+        <v>730059314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -1836,10 +2086,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1891,6 +2141,17 @@
       </c>
       <c r="D4" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2743,6 +3004,157 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75209924-C3A2-4B36-BD60-A81741FEAB56}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="str" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P1),LEN(CELL("filename",P1))-FIND("]",CELL("filename",P1))),"_Event_", ProductionData[[#This Row],[Name]])</f>
+        <v>DT_ProductionData_Event_TargetRateChanged</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P2),LEN(CELL("filename",P2))-FIND("]",CELL("filename",P2))),"_Event_", ProductionData[[#This Row],[Name]])</f>
+        <v>DT_ProductionData_Event_ShiftCompleted</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P3),LEN(CELL("filename",P3))-FIND("]",CELL("filename",P3))),"_Event_", ProductionData[[#This Row],[Name]])</f>
+        <v>DT_ProductionData_Event_BehindScheduleAcceptable</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xlfn.CONCAT("DT_", RIGHT(CELL("filename",P4),LEN(CELL("filename",P4))-FIND("]",CELL("filename",P4))),"_Event_", ProductionData[[#This Row],[Name]])</f>
+        <v>DT_ProductionData_Event_BehindScheduleWarning</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{04C4F3F4-B798-4F29-887A-B5E01DB39E23}">
+            <xm:f>IF(IFERROR(MATCH(D3,Translations!$A$2:$A$1000,0),FALSE),FALSE,TRUE)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC8C8"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D3:D6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B49675A-B785-4340-B070-972FE3EC25B2}">
+          <x14:formula1>
+            <xm:f>Helper!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2878,7 +3290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -3044,7 +3456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -3091,144 +3503,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>1998170941</v>
-      </c>
-      <c r="C2">
-        <v>-1925411841</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3">
-        <v>1054446003</v>
-      </c>
-      <c r="C3">
-        <v>662966212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4">
-        <v>1691620521</v>
-      </c>
-      <c r="C4">
-        <v>1845685619</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>2038111688</v>
-      </c>
-      <c r="C5">
-        <v>46465576</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6">
-        <v>-1810971161</v>
-      </c>
-      <c r="C6">
-        <v>1659002869</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7">
-        <v>-668640524</v>
-      </c>
-      <c r="C7">
-        <v>-1957413921</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B8">
-        <v>-1476574130</v>
-      </c>
-      <c r="C8">
-        <v>-97488637</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9">
-        <v>1259079353</v>
-      </c>
-      <c r="C9">
-        <v>-1307371275</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10">
-        <v>1688958672</v>
-      </c>
-      <c r="C10">
-        <v>-1307371275</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B11">
-        <v>-1825382818</v>
-      </c>
-      <c r="C11">
-        <v>-1307371275</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>